<commit_message>
made changes to excel file. comments added
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -46,7 +46,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -86,25 +86,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -414,27 +402,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finised grade maker 2000need to comment
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -46,7 +46,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -86,13 +86,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -402,27 +414,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
tried to do more - finish swimmy
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -414,14 +414,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
can explore list in a 2d array fixxed adding new lines
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,58 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -60,18 +45,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -150,7 +211,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -185,7 +245,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -220,16 +279,20 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -351,77 +414,74 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="str">
-        <v>Name</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Mark</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Max Marks</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Grade</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Percentage</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Mark</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Max Marks</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Grade</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>tony</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>11</v>
+      </c>
+      <c r="C2" t="n">
+        <v>20</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E1"/>
-  </ignoredErrors>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>